<commit_message>
Gmean and method ok
</commit_message>
<xml_diff>
--- a/data/ecoinvent_geometric_mean.xlsx
+++ b/data/ecoinvent_geometric_mean.xlsx
@@ -2425,18 +2425,18 @@
     <t>iron to soil (unspecified)</t>
   </si>
   <si>
+    <t>iron, ion to water groundwater</t>
+  </si>
+  <si>
+    <t>iron, 46% in ore, 25% in crude ore to raw (unspecified)</t>
+  </si>
+  <si>
+    <t>iron, 72% in magnetite, 14% in crude ore to raw (unspecified)</t>
+  </si>
+  <si>
     <t>iron to water groundwater</t>
   </si>
   <si>
-    <t>iron, 46% in ore, 25% in crude ore to raw (unspecified)</t>
-  </si>
-  <si>
-    <t>iron, 72% in magnetite, 14% in crude ore to raw (unspecified)</t>
-  </si>
-  <si>
-    <t>iron, ion to water groundwater</t>
-  </si>
-  <si>
     <t>iron, ion to water groundwater, long-term</t>
   </si>
   <si>
@@ -3628,12 +3628,12 @@
     <t>potassium to soil (unspecified)</t>
   </si>
   <si>
+    <t>potassium, ion to water groundwater</t>
+  </si>
+  <si>
     <t>potassium to water groundwater</t>
   </si>
   <si>
-    <t>potassium, ion to water groundwater</t>
-  </si>
-  <si>
     <t>potassium, ion to water groundwater, long-term</t>
   </si>
   <si>
@@ -4144,10 +4144,10 @@
     <t>sodium to soil (unspecified)</t>
   </si>
   <si>
+    <t>sodium, ion to water groundwater</t>
+  </si>
+  <si>
     <t>sodium to water groundwater</t>
-  </si>
-  <si>
-    <t>sodium, ion to water groundwater</t>
   </si>
   <si>
     <t>sodium, ion to water groundwater, long-term</t>

</xml_diff>